<commit_message>
0.75 DC / 9% EEC / ORPoffset / Pr.Payroll / Crises in 2022
</commit_message>
<xml_diff>
--- a/Model Inputs 2020.xlsx
+++ b/Model Inputs 2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swaro\Desktop\South Carolina\South Carolina Model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anilniraula/Dropbox/My Mac (Anils-MacBook-Pro.local)/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{060FA33B-66B1-47E3-A5C1-DD0DBFAB9F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C014EB83-3C22-F244-8975-010B82EA2AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30645" yWindow="1830" windowWidth="17250" windowHeight="8865" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20100" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Numeric Inputs" sheetId="1" r:id="rId1"/>
@@ -1451,20 +1451,20 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>87</v>
       </c>
@@ -1486,7 +1486,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>7.2499999999999995E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>89</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1519,12 +1519,12 @@
         <v>2.2499999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="50" t="s">
         <v>186</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="50" t="s">
         <v>187</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
         <v>190</v>
       </c>
@@ -1557,7 +1557,7 @@
         <v>2.1399999999999999E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>2021</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="53" t="s">
         <v>192</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>0.11691702481432163</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="53" t="s">
         <v>193</v>
       </c>
@@ -1601,7 +1601,7 @@
         <v>9.3299999999999994E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="53" t="s">
         <v>194</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>9.3299999999999994E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>99</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>1.1999999999999999E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="50" t="s">
         <v>210</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="53" t="s">
         <v>211</v>
       </c>
@@ -1645,7 +1645,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="53" t="s">
         <v>212</v>
       </c>
@@ -1656,7 +1656,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="53" t="s">
         <v>213</v>
       </c>
@@ -1667,7 +1667,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -1678,7 +1678,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="53" t="s">
         <v>218</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>97</v>
       </c>
@@ -1700,7 +1700,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>220</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>221</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>8.9999999999999993E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>235</v>
       </c>
@@ -1755,13 +1755,13 @@
         <v>1.1386456406995427E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="41" t="s">
         <v>6</v>
       </c>
       <c r="C29" s="42"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -1784,7 +1784,7 @@
         <v>99.99</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -1817,7 +1817,7 @@
         <v>11.362052951411172</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -1828,7 +1828,7 @@
         <v>0.78425225741758364</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>19</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>22.724105902822345</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>172</v>
       </c>
@@ -1852,7 +1852,7 @@
         <v>22.724105902822345</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>173</v>
       </c>
@@ -1864,7 +1864,7 @@
         <v>11.362052951411172</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>174</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>0.25249006558691495</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>7.609863E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>80</v>
       </c>
@@ -1898,7 +1898,7 @@
         <v>6.7256999999999997E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -1919,23 +1919,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>90</v>
       </c>
@@ -1946,7 +1946,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>108</v>
       </c>
@@ -1957,7 +1957,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>91</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>263</v>
       </c>
@@ -2001,12 +2001,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>241</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>242</v>
       </c>
@@ -2028,7 +2028,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>245</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>113</v>
       </c>
@@ -2050,7 +2050,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>268</v>
       </c>
@@ -2061,12 +2061,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="41" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -2201,14 +2201,14 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="26" t="s">
         <v>22</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="26" t="s">
         <v>23</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="26" t="s">
         <v>20</v>
       </c>
@@ -2266,7 +2266,7 @@
       <c r="K4" s="26"/>
       <c r="L4" s="26"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="26" t="s">
         <v>21</v>
       </c>
@@ -2285,7 +2285,7 @@
       </c>
       <c r="L5" s="26"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="26" t="s">
         <v>24</v>
       </c>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="L6" s="26"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="26" t="s">
         <v>25</v>
       </c>
@@ -2321,7 +2321,7 @@
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="26" t="s">
         <v>49</v>
       </c>
@@ -2342,7 +2342,7 @@
       <c r="K8" s="26"/>
       <c r="L8" s="26"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="26" t="s">
         <v>26</v>
       </c>
@@ -2358,7 +2358,7 @@
       <c r="K9" s="26"/>
       <c r="L9" s="26"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="26" t="s">
         <v>27</v>
       </c>
@@ -2367,7 +2367,7 @@
       <c r="K10" s="26"/>
       <c r="L10" s="26"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="26" t="s">
         <v>28</v>
       </c>
@@ -2385,7 +2385,7 @@
       <c r="K11" s="26"/>
       <c r="L11" s="26"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C12" s="45" t="s">
         <v>183</v>
       </c>
@@ -2399,13 +2399,13 @@
       <c r="K12" s="26"/>
       <c r="L12" s="26"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G13" s="45"/>
       <c r="I13" s="26"/>
       <c r="K13" s="26"/>
       <c r="L13" s="26"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C14" s="45" t="s">
         <v>105</v>
       </c>
@@ -2413,13 +2413,13 @@
       <c r="K14" s="26"/>
       <c r="L14" s="26"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C15" s="45" t="s">
         <v>106</v>
       </c>
       <c r="L15" s="26"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="L16" s="26"/>
     </row>
   </sheetData>
@@ -2435,18 +2435,18 @@
       <selection activeCell="BM2" sqref="BM2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="12" width="8.33203125" customWidth="1"/>
     <col min="13" max="13" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.6640625" bestFit="1" customWidth="1"/>
@@ -2456,51 +2456,51 @@
     <col min="26" max="26" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="32" width="7.5546875" customWidth="1"/>
-    <col min="33" max="33" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="35" width="7.5546875" customWidth="1"/>
-    <col min="36" max="36" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="7.5" customWidth="1"/>
+    <col min="33" max="33" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="34" max="35" width="7.5" customWidth="1"/>
+    <col min="36" max="36" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="37" max="38" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="39" max="40" width="8.33203125" customWidth="1"/>
-    <col min="45" max="45" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="47" max="66" width="14.33203125" customWidth="1"/>
-    <col min="67" max="67" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="68" max="70" width="11.5546875" customWidth="1"/>
+    <col min="67" max="67" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="68" max="70" width="11.5" customWidth="1"/>
     <col min="71" max="71" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="72" max="72" width="8.6640625" customWidth="1"/>
-    <col min="73" max="73" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="74" max="76" width="9.44140625" customWidth="1"/>
+    <col min="73" max="73" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="74" max="76" width="9.5" customWidth="1"/>
     <col min="77" max="77" width="6" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="18.44140625" customWidth="1"/>
-    <col min="81" max="81" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="15.88671875" customWidth="1"/>
-    <col min="83" max="85" width="11.88671875" customWidth="1"/>
+    <col min="78" max="78" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="18.5" customWidth="1"/>
+    <col min="81" max="81" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="15.83203125" customWidth="1"/>
+    <col min="83" max="85" width="11.83203125" customWidth="1"/>
     <col min="86" max="86" width="22" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="89" max="90" width="11.5546875" customWidth="1"/>
+    <col min="87" max="87" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="89" max="90" width="11.5" customWidth="1"/>
     <col min="91" max="91" width="12" bestFit="1" customWidth="1"/>
     <col min="92" max="92" width="12" customWidth="1"/>
     <col min="93" max="93" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="94" max="94" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="95" max="95" width="21.5" bestFit="1" customWidth="1"/>
     <col min="96" max="96" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="97" max="97" width="12" bestFit="1" customWidth="1"/>
     <col min="98" max="98" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="99" max="99" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="100" max="100" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="100" max="100" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="101" max="101" width="12" bestFit="1" customWidth="1"/>
     <col min="102" max="102" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="103" max="103" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="104" max="104" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="2" spans="1:113" s="29" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:113" s="29" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>2019</v>
       </c>
@@ -3095,7 +3095,7 @@
       <c r="DH2" s="49"/>
       <c r="DI2" s="49"/>
     </row>
-    <row r="3" spans="1:113" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:113" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -3322,20 +3322,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J62"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="12.44140625" customWidth="1"/>
-    <col min="6" max="6" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>37</v>
       </c>
@@ -3367,7 +3367,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>5.8400000000000001E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -3431,39 +3431,39 @@
         <v>-1.5800000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2021</v>
       </c>
-      <c r="B4" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="C4" s="15">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="D4" s="15">
-        <v>0.06</v>
-      </c>
-      <c r="E4" s="15">
-        <v>7.0000000000000007E-2</v>
+      <c r="B4" s="16">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.28599999999999998</v>
       </c>
       <c r="F4" s="16">
-        <v>-0.24</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="G4" s="16">
-        <v>-0.24</v>
-      </c>
-      <c r="H4" s="17">
-        <v>0.05</v>
-      </c>
-      <c r="I4" s="17">
-        <v>9.0000000000000011E-2</v>
-      </c>
-      <c r="J4" s="17">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="H4" s="16">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="I4" s="16">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="J4" s="16">
+        <v>0.28599999999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -3479,11 +3479,11 @@
       <c r="E5" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F5" s="18">
-        <v>0.11</v>
-      </c>
-      <c r="G5" s="18">
-        <v>0.11</v>
+      <c r="F5" s="16">
+        <v>-0.24</v>
+      </c>
+      <c r="G5" s="16">
+        <v>-0.24</v>
       </c>
       <c r="H5" s="17">
         <v>0.05</v>
@@ -3495,7 +3495,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -3527,12 +3527,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2024</v>
       </c>
-      <c r="B7">
-        <v>4.0000000000000001E-3</v>
+      <c r="B7" s="15">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C7" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3559,12 +3559,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2025</v>
       </c>
       <c r="B8">
-        <v>0.19</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="C8" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3575,11 +3575,11 @@
       <c r="E8" s="15">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F8" s="19">
-        <v>0.06</v>
-      </c>
-      <c r="G8" s="19">
-        <v>0.06</v>
+      <c r="F8" s="18">
+        <v>0.11</v>
+      </c>
+      <c r="G8" s="18">
+        <v>0.11</v>
       </c>
       <c r="H8" s="17">
         <v>0.05</v>
@@ -3591,12 +3591,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2026</v>
       </c>
       <c r="B9">
-        <v>0.16700000000000001</v>
+        <v>0.19</v>
       </c>
       <c r="C9" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3623,12 +3623,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2027</v>
       </c>
       <c r="B10">
-        <v>0.19309999999999999</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="C10" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3655,12 +3655,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2028</v>
       </c>
       <c r="B11">
-        <v>0.19009999999999999</v>
+        <v>0.19309999999999999</v>
       </c>
       <c r="C11" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3687,12 +3687,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2029</v>
       </c>
       <c r="B12">
-        <v>0.1482</v>
+        <v>0.19009999999999999</v>
       </c>
       <c r="C12" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3719,12 +3719,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2030</v>
       </c>
       <c r="B13">
-        <v>0.114</v>
+        <v>0.1482</v>
       </c>
       <c r="C13" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3751,12 +3751,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2031</v>
       </c>
       <c r="B14">
-        <v>-0.111</v>
+        <v>0.114</v>
       </c>
       <c r="C14" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3773,22 +3773,22 @@
       <c r="G14" s="19">
         <v>0.06</v>
       </c>
-      <c r="H14" s="20">
-        <v>8.0142406836996249E-2</v>
-      </c>
-      <c r="I14" s="20">
-        <v>6.0138038441437391E-2</v>
+      <c r="H14" s="17">
+        <v>0.05</v>
+      </c>
+      <c r="I14" s="17">
+        <v>9.0000000000000011E-2</v>
       </c>
       <c r="J14" s="17">
         <v>0.06</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2032</v>
       </c>
       <c r="B15">
-        <v>-8.7999999999999995E-2</v>
+        <v>-0.111</v>
       </c>
       <c r="C15" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3815,12 +3815,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2033</v>
       </c>
       <c r="B16">
-        <v>2.7E-2</v>
+        <v>-8.7999999999999995E-2</v>
       </c>
       <c r="C16" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3847,12 +3847,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2034</v>
       </c>
       <c r="B17">
-        <v>0.153</v>
+        <v>2.7E-2</v>
       </c>
       <c r="C17" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3879,12 +3879,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2035</v>
       </c>
       <c r="B18">
-        <v>9.6000000000000002E-2</v>
+        <v>0.153</v>
       </c>
       <c r="C18" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3911,12 +3911,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2036</v>
       </c>
-      <c r="B19" s="21">
-        <v>0.12</v>
+      <c r="B19">
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="C19" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3930,8 +3930,8 @@
       <c r="F19" s="19">
         <v>0.06</v>
       </c>
-      <c r="G19" s="18">
-        <v>-0.24</v>
+      <c r="G19" s="19">
+        <v>0.06</v>
       </c>
       <c r="H19" s="20">
         <v>8.0142406836996249E-2</v>
@@ -3943,12 +3943,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2037</v>
       </c>
       <c r="B20" s="21">
-        <v>0.16700000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="C20" s="15">
         <v>7.0000000000000007E-2</v>
@@ -3963,7 +3963,7 @@
         <v>0.06</v>
       </c>
       <c r="G20" s="18">
-        <v>0.11</v>
+        <v>-0.24</v>
       </c>
       <c r="H20" s="20">
         <v>8.0142406836996249E-2</v>
@@ -3975,12 +3975,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2038</v>
       </c>
       <c r="B21" s="21">
-        <v>-0.06</v>
+        <v>0.16700000000000001</v>
       </c>
       <c r="C21" s="15">
         <v>7.0000000000000007E-2</v>
@@ -4007,15 +4007,15 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2039</v>
       </c>
       <c r="B22" s="21">
-        <v>-0.17699999999999999</v>
-      </c>
-      <c r="C22" s="22">
-        <v>9.2999999999999999E-2</v>
+        <v>-0.06</v>
+      </c>
+      <c r="C22" s="15">
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="D22" s="15">
         <v>0.06</v>
@@ -4039,15 +4039,15 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2040</v>
       </c>
       <c r="B23" s="21">
-        <v>0.17699999999999999</v>
+        <v>-0.17699999999999999</v>
       </c>
       <c r="C23" s="22">
-        <v>2.1999999999999999E-2</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="D23" s="15">
         <v>0.06</v>
@@ -4058,8 +4058,8 @@
       <c r="F23" s="19">
         <v>0.06</v>
       </c>
-      <c r="G23" s="19">
-        <v>0.06</v>
+      <c r="G23" s="18">
+        <v>0.11</v>
       </c>
       <c r="H23" s="20">
         <v>8.0142406836996249E-2</v>
@@ -4071,15 +4071,15 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2041</v>
       </c>
-      <c r="B24" s="23">
-        <v>0.19</v>
+      <c r="B24" s="21">
+        <v>0.17699999999999999</v>
       </c>
       <c r="C24" s="22">
-        <v>0.02</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D24" s="15">
         <v>0.06</v>
@@ -4103,15 +4103,15 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2042</v>
       </c>
       <c r="B25" s="23">
-        <v>1.6E-2</v>
+        <v>0.19</v>
       </c>
       <c r="C25" s="22">
-        <v>4.2000000000000003E-2</v>
+        <v>0.02</v>
       </c>
       <c r="D25" s="15">
         <v>0.06</v>
@@ -4135,15 +4135,15 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2043</v>
       </c>
       <c r="B26" s="23">
-        <v>0.108</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C26" s="22">
-        <v>2.1999999999999999E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="D26" s="15">
         <v>0.06</v>
@@ -4167,15 +4167,15 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2044</v>
       </c>
       <c r="B27" s="23">
-        <v>0.14199999999999999</v>
-      </c>
-      <c r="C27" s="15">
-        <v>7.0000000000000007E-2</v>
+        <v>0.108</v>
+      </c>
+      <c r="C27" s="22">
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="D27" s="15">
         <v>0.06</v>
@@ -4199,12 +4199,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2045</v>
       </c>
       <c r="B28" s="23">
-        <v>3.6999999999999998E-2</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="C28" s="15">
         <v>7.0000000000000007E-2</v>
@@ -4231,12 +4231,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2046</v>
       </c>
       <c r="B29" s="23">
-        <v>3.1E-2</v>
+        <v>3.6999999999999998E-2</v>
       </c>
       <c r="C29" s="15">
         <v>7.0000000000000007E-2</v>
@@ -4263,12 +4263,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2047</v>
       </c>
       <c r="B30" s="23">
-        <v>0.11799999999999999</v>
+        <v>3.1E-2</v>
       </c>
       <c r="C30" s="15">
         <v>7.0000000000000007E-2</v>
@@ -4295,12 +4295,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2048</v>
       </c>
       <c r="B31" s="23">
-        <v>7.1999999999999995E-2</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="C31" s="15">
         <v>7.0000000000000007E-2</v>
@@ -4327,12 +4327,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2049</v>
       </c>
       <c r="B32" s="23">
-        <v>6.2799999999999995E-2</v>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="C32" s="15">
         <v>7.0000000000000007E-2</v>
@@ -4359,12 +4359,12 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2050</v>
       </c>
       <c r="B33" s="23">
-        <v>-9.7000000000000003E-3</v>
+        <v>6.2799999999999995E-2</v>
       </c>
       <c r="C33" s="15">
         <v>7.0000000000000007E-2</v>
@@ -4391,7 +4391,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2051</v>
       </c>
@@ -4423,7 +4423,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2052</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2053</v>
       </c>
@@ -4478,16 +4478,16 @@
         <v>0.06</v>
       </c>
       <c r="H36" s="20">
-        <v>8.0142406836996194E-2</v>
+        <v>8.0142406836996249E-2</v>
       </c>
       <c r="I36" s="20">
-        <v>6.0138038441437398E-2</v>
+        <v>6.0138038441437391E-2</v>
       </c>
       <c r="J36" s="17">
         <v>0.06</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2054</v>
       </c>
@@ -4519,7 +4519,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2055</v>
       </c>
@@ -4551,7 +4551,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2056</v>
       </c>
@@ -4583,7 +4583,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2057</v>
       </c>
@@ -4615,7 +4615,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2058</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2059</v>
       </c>
@@ -4679,7 +4679,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2060</v>
       </c>
@@ -4711,7 +4711,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2061</v>
       </c>
@@ -4743,7 +4743,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2062</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2063</v>
       </c>
@@ -4807,7 +4807,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2064</v>
       </c>
@@ -4839,7 +4839,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2065</v>
       </c>
@@ -4871,7 +4871,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2066</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2067</v>
       </c>
@@ -4935,7 +4935,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2068</v>
       </c>
@@ -4967,7 +4967,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2069</v>
       </c>
@@ -4999,7 +4999,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2070</v>
       </c>
@@ -5031,7 +5031,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2071</v>
       </c>
@@ -5063,7 +5063,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2072</v>
       </c>
@@ -5095,7 +5095,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2073</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2074</v>
       </c>
@@ -5159,7 +5159,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2075</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2076</v>
       </c>
@@ -5223,7 +5223,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2077</v>
       </c>
@@ -5255,7 +5255,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2078</v>
       </c>
@@ -5287,7 +5287,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2079</v>
       </c>
@@ -5332,9 +5332,9 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -5342,7 +5342,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -5350,7 +5350,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -5366,7 +5366,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2023</v>
       </c>
@@ -5374,7 +5374,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2024</v>
       </c>
@@ -5382,7 +5382,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -5390,7 +5390,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2026</v>
       </c>
@@ -5398,7 +5398,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2027</v>
       </c>
@@ -5406,7 +5406,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2028</v>
       </c>
@@ -5414,7 +5414,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2029</v>
       </c>
@@ -5422,7 +5422,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2030</v>
       </c>
@@ -5430,7 +5430,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2031</v>
       </c>
@@ -5438,7 +5438,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2032</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2033</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2034</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2035</v>
       </c>
@@ -5470,7 +5470,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2036</v>
       </c>
@@ -5478,7 +5478,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2037</v>
       </c>
@@ -5486,7 +5486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2038</v>
       </c>
@@ -5494,7 +5494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2039</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2040</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2041</v>
       </c>
@@ -5518,7 +5518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2042</v>
       </c>
@@ -5526,7 +5526,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2043</v>
       </c>
@@ -5534,7 +5534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2044</v>
       </c>
@@ -5542,7 +5542,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2045</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2046</v>
       </c>
@@ -5558,7 +5558,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2047</v>
       </c>
@@ -5566,7 +5566,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2048</v>
       </c>
@@ -5574,7 +5574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2049</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2050</v>
       </c>
@@ -5590,7 +5590,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2051</v>
       </c>
@@ -5598,7 +5598,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2052</v>
       </c>
@@ -5606,7 +5606,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2053</v>
       </c>
@@ -5614,7 +5614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2054</v>
       </c>
@@ -5622,7 +5622,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2055</v>
       </c>
@@ -5630,7 +5630,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2056</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2057</v>
       </c>
@@ -5646,7 +5646,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2058</v>
       </c>
@@ -5654,7 +5654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2059</v>
       </c>
@@ -5662,7 +5662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2060</v>
       </c>
@@ -5670,7 +5670,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2061</v>
       </c>
@@ -5678,7 +5678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2062</v>
       </c>
@@ -5686,7 +5686,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2063</v>
       </c>
@@ -5694,7 +5694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2064</v>
       </c>
@@ -5702,7 +5702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2065</v>
       </c>
@@ -5710,7 +5710,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2066</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2067</v>
       </c>
@@ -5726,7 +5726,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2068</v>
       </c>
@@ -5734,7 +5734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2069</v>
       </c>
@@ -5742,7 +5742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2070</v>
       </c>
@@ -5750,7 +5750,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2071</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2072</v>
       </c>
@@ -5766,7 +5766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2073</v>
       </c>
@@ -5774,7 +5774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2074</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2075</v>
       </c>
@@ -5790,7 +5790,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2076</v>
       </c>
@@ -5798,7 +5798,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2077</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2078</v>
       </c>
@@ -5814,7 +5814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2079</v>
       </c>
@@ -5822,7 +5822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2080</v>
       </c>
@@ -5843,9 +5843,9 @@
       <selection activeCell="B2" sqref="B2:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -5853,7 +5853,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2020</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2021</v>
       </c>
@@ -5869,7 +5869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2022</v>
       </c>
@@ -5877,7 +5877,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2023</v>
       </c>
@@ -5885,7 +5885,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2024</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2025</v>
       </c>
@@ -5901,7 +5901,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2026</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2027</v>
       </c>
@@ -5917,7 +5917,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2028</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2029</v>
       </c>
@@ -5933,7 +5933,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2030</v>
       </c>
@@ -5941,7 +5941,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2031</v>
       </c>
@@ -5949,7 +5949,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2032</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2033</v>
       </c>
@@ -5965,7 +5965,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2034</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2035</v>
       </c>
@@ -5981,7 +5981,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2036</v>
       </c>
@@ -5989,7 +5989,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2037</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2038</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2039</v>
       </c>
@@ -6013,7 +6013,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2040</v>
       </c>
@@ -6021,7 +6021,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2041</v>
       </c>
@@ -6029,7 +6029,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2042</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2043</v>
       </c>
@@ -6045,7 +6045,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2044</v>
       </c>
@@ -6053,7 +6053,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2045</v>
       </c>
@@ -6061,7 +6061,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2046</v>
       </c>
@@ -6069,7 +6069,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2047</v>
       </c>
@@ -6077,7 +6077,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2048</v>
       </c>
@@ -6085,7 +6085,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2049</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2050</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2051</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2052</v>
       </c>
@@ -6117,7 +6117,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2053</v>
       </c>
@@ -6125,7 +6125,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2054</v>
       </c>
@@ -6133,7 +6133,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2055</v>
       </c>
@@ -6141,7 +6141,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2056</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2057</v>
       </c>
@@ -6157,7 +6157,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2058</v>
       </c>
@@ -6165,7 +6165,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2059</v>
       </c>
@@ -6173,7 +6173,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2060</v>
       </c>
@@ -6181,7 +6181,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2061</v>
       </c>
@@ -6189,7 +6189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2062</v>
       </c>
@@ -6197,7 +6197,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2063</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2064</v>
       </c>
@@ -6213,7 +6213,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2065</v>
       </c>
@@ -6221,7 +6221,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2066</v>
       </c>
@@ -6229,7 +6229,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2067</v>
       </c>
@@ -6237,7 +6237,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2068</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2069</v>
       </c>
@@ -6253,7 +6253,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2070</v>
       </c>
@@ -6261,7 +6261,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2071</v>
       </c>
@@ -6269,7 +6269,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2072</v>
       </c>
@@ -6277,7 +6277,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2073</v>
       </c>
@@ -6285,7 +6285,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2074</v>
       </c>
@@ -6293,7 +6293,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2075</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2076</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2077</v>
       </c>
@@ -6317,7 +6317,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2078</v>
       </c>
@@ -6325,7 +6325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2079</v>
       </c>
@@ -6333,7 +6333,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2080</v>
       </c>
@@ -6354,7 +6354,7 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
@@ -6362,7 +6362,7 @@
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -6379,7 +6379,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>-2.989999860820932E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>-0.14371932664345946</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2025</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>-0.3172090852344927</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2026</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>-0.56632395350531439</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2027</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>-0.89740564940072887</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2028</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>-1.3171671419079198</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2029</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>-1.8327109828897741</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2030</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>-2.4515484576317759</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2031</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>-3.2952488593257501</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2032</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>-4.1613564139224808</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2033</v>
       </c>
@@ -6636,7 +6636,7 @@
         <v>-5.3041689190959387</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2034</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>-6.6221745292955383</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2035</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>-7.943436309859357</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2036</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>-9.6307415467693751</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2037</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>-11.532739820329681</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2038</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>-13.664412252479506</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2039</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>-16.04155415217506</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2040</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>-18.680813639903807</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2041</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>-21.599731954590361</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2042</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>-24.467253321696223</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2043</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>-27.973410722695299</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2044</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>-31.408343949274922</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2045</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>-34.699545327336189</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2046</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>-38.710713461928201</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2047</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>-42.546378667759505</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2048</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>-46.660816086735032</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2049</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>-51.069804111245524</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2050</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>-55.789892066981835</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2051</v>
       </c>
@@ -6955,12 +6955,12 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -6974,7 +6974,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2019</v>
       </c>
@@ -6988,7 +6988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2020</v>
       </c>
@@ -7002,7 +7002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2021</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2022</v>
       </c>
@@ -7030,7 +7030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2023</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -7058,7 +7058,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2025</v>
       </c>
@@ -7072,7 +7072,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2026</v>
       </c>
@@ -7086,7 +7086,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2027</v>
       </c>
@@ -7100,7 +7100,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2028</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2029</v>
       </c>
@@ -7128,7 +7128,7 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2030</v>
       </c>
@@ -7142,7 +7142,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2031</v>
       </c>
@@ -7156,7 +7156,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2032</v>
       </c>
@@ -7170,7 +7170,7 @@
         <v>0.32</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2033</v>
       </c>
@@ -7184,7 +7184,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2034</v>
       </c>
@@ -7198,7 +7198,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2035</v>
       </c>
@@ -7212,7 +7212,7 @@
         <v>0.43</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2036</v>
       </c>
@@ -7226,7 +7226,7 @@
         <v>0.47</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2037</v>
       </c>
@@ -7240,7 +7240,7 @@
         <v>0.51</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2038</v>
       </c>
@@ -7254,7 +7254,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2039</v>
       </c>
@@ -7268,7 +7268,7 @@
         <v>0.59</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2040</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>0.63</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2041</v>
       </c>
@@ -7296,7 +7296,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2042</v>
       </c>
@@ -7310,7 +7310,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2043</v>
       </c>
@@ -7324,7 +7324,7 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2044</v>
       </c>
@@ -7338,7 +7338,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2045</v>
       </c>
@@ -7352,7 +7352,7 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2046</v>
       </c>
@@ -7366,7 +7366,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2047</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>0.84</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2048</v>
       </c>
@@ -7394,7 +7394,7 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2049</v>
       </c>
@@ -7408,7 +7408,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2050</v>
       </c>
@@ -7422,7 +7422,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2051</v>
       </c>

</xml_diff>